<commit_message>
Init setup of backend (sleepy)
</commit_message>
<xml_diff>
--- a/ID_zespolu_ewidencja.xlsx
+++ b/ID_zespolu_ewidencja.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mskrzyp\Desktop\Github\e.leclerc\s5-Android-APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2F6968-E2B4-4959-BCBD-0B085B184409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BC889B-B07B-4924-8F8B-F3A8695CA815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="345" windowWidth="21150" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1_Mateusz_Skrzypek" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>Data</t>
   </si>
@@ -60,16 +60,19 @@
     <t>Narastająco</t>
   </si>
   <si>
-    <t>Research, talk with specialist</t>
-  </si>
-  <si>
     <t>Initial research</t>
   </si>
   <si>
-    <t xml:space="preserve">11-18, 19-21:11, api sketch, </t>
+    <t>Api sketch</t>
   </si>
   <si>
-    <t>12-17 api, usecases, 17-20</t>
+    <t>Talk with backend specialist</t>
+  </si>
+  <si>
+    <t>Usecase diagram - functionality call</t>
+  </si>
+  <si>
+    <t>Backend alternatives</t>
   </si>
 </sst>
 </file>
@@ -509,7 +512,7 @@
   <dimension ref="A1:D132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B5:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +545,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1">
         <f>SUM(B2)</f>
@@ -575,7 +578,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
@@ -590,7 +593,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
@@ -602,23 +605,29 @@
         <v>45571</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>8.5</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45572</v>
       </c>
+      <c r="B8">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -627,7 +636,7 @@
       </c>
       <c r="D9" s="1">
         <f>B9+D8</f>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -636,7 +645,7 @@
       </c>
       <c r="D10" s="1">
         <f>B10+D9</f>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -645,7 +654,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -654,7 +663,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,7 +672,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -672,7 +681,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -681,7 +690,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -690,7 +699,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -699,7 +708,7 @@
       </c>
       <c r="D17" s="1">
         <f>B17+D16</f>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -708,7 +717,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -717,7 +726,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -726,7 +735,7 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -735,7 +744,7 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -744,7 +753,7 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -753,7 +762,7 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -762,7 +771,7 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,7 +780,7 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -780,7 +789,7 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -789,7 +798,7 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -798,7 +807,7 @@
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -807,7 +816,7 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -816,7 +825,7 @@
       </c>
       <c r="D30" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -825,7 +834,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -834,7 +843,7 @@
       </c>
       <c r="D32" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -843,7 +852,7 @@
       </c>
       <c r="D33" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -852,7 +861,7 @@
       </c>
       <c r="D34" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -861,7 +870,7 @@
       </c>
       <c r="D35" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -870,7 +879,7 @@
       </c>
       <c r="D36" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -879,7 +888,7 @@
       </c>
       <c r="D37" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -888,7 +897,7 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -897,7 +906,7 @@
       </c>
       <c r="D39" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -906,7 +915,7 @@
       </c>
       <c r="D40" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -915,7 +924,7 @@
       </c>
       <c r="D41" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -924,7 +933,7 @@
       </c>
       <c r="D42" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -933,7 +942,7 @@
       </c>
       <c r="D43" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -942,7 +951,7 @@
       </c>
       <c r="D44" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -951,7 +960,7 @@
       </c>
       <c r="D45" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -960,7 +969,7 @@
       </c>
       <c r="D46" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -969,7 +978,7 @@
       </c>
       <c r="D47" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -978,7 +987,7 @@
       </c>
       <c r="D48" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -987,7 +996,7 @@
       </c>
       <c r="D49" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -996,7 +1005,7 @@
       </c>
       <c r="D50" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1005,7 +1014,7 @@
       </c>
       <c r="D51" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1014,7 +1023,7 @@
       </c>
       <c r="D52" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,7 +1032,7 @@
       </c>
       <c r="D53" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1032,7 +1041,7 @@
       </c>
       <c r="D54" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1041,7 +1050,7 @@
       </c>
       <c r="D55" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1050,7 +1059,7 @@
       </c>
       <c r="D56" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1059,7 +1068,7 @@
       </c>
       <c r="D57" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1068,7 +1077,7 @@
       </c>
       <c r="D58" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1077,7 +1086,7 @@
       </c>
       <c r="D59" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1086,7 +1095,7 @@
       </c>
       <c r="D60" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1095,7 +1104,7 @@
       </c>
       <c r="D61" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1104,7 +1113,7 @@
       </c>
       <c r="D62" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1113,7 +1122,7 @@
       </c>
       <c r="D63" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1122,7 +1131,7 @@
       </c>
       <c r="D64" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1131,7 +1140,7 @@
       </c>
       <c r="D65" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1140,7 +1149,7 @@
       </c>
       <c r="D66" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1149,7 +1158,7 @@
       </c>
       <c r="D67" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1158,7 +1167,7 @@
       </c>
       <c r="D68" s="1">
         <f t="shared" ref="D68:D127" si="1">B68+D67</f>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1167,7 +1176,7 @@
       </c>
       <c r="D69" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1176,7 +1185,7 @@
       </c>
       <c r="D70" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1185,7 +1194,7 @@
       </c>
       <c r="D71" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1194,7 +1203,7 @@
       </c>
       <c r="D72" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1203,7 +1212,7 @@
       </c>
       <c r="D73" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1212,7 +1221,7 @@
       </c>
       <c r="D74" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1221,7 +1230,7 @@
       </c>
       <c r="D75" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,7 +1239,7 @@
       </c>
       <c r="D76" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1239,7 +1248,7 @@
       </c>
       <c r="D77" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1248,7 +1257,7 @@
       </c>
       <c r="D78" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1257,7 +1266,7 @@
       </c>
       <c r="D79" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1266,7 +1275,7 @@
       </c>
       <c r="D80" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1275,7 +1284,7 @@
       </c>
       <c r="D81" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1284,7 +1293,7 @@
       </c>
       <c r="D82" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1293,7 +1302,7 @@
       </c>
       <c r="D83" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1302,7 +1311,7 @@
       </c>
       <c r="D84" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,7 +1320,7 @@
       </c>
       <c r="D85" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1320,7 +1329,7 @@
       </c>
       <c r="D86" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1329,7 +1338,7 @@
       </c>
       <c r="D87" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1338,7 +1347,7 @@
       </c>
       <c r="D88" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1347,7 +1356,7 @@
       </c>
       <c r="D89" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1356,7 +1365,7 @@
       </c>
       <c r="D90" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1365,7 +1374,7 @@
       </c>
       <c r="D91" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -1374,7 +1383,7 @@
       </c>
       <c r="D92" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1383,7 +1392,7 @@
       </c>
       <c r="D93" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -1392,7 +1401,7 @@
       </c>
       <c r="D94" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -1401,7 +1410,7 @@
       </c>
       <c r="D95" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -1410,7 +1419,7 @@
       </c>
       <c r="D96" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1419,7 +1428,7 @@
       </c>
       <c r="D97" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1428,7 +1437,7 @@
       </c>
       <c r="D98" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1437,7 +1446,7 @@
       </c>
       <c r="D99" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -1446,7 +1455,7 @@
       </c>
       <c r="D100" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1455,7 +1464,7 @@
       </c>
       <c r="D101" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -1464,7 +1473,7 @@
       </c>
       <c r="D102" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -1473,7 +1482,7 @@
       </c>
       <c r="D103" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -1482,7 +1491,7 @@
       </c>
       <c r="D104" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -1491,7 +1500,7 @@
       </c>
       <c r="D105" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -1500,7 +1509,7 @@
       </c>
       <c r="D106" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -1509,7 +1518,7 @@
       </c>
       <c r="D107" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -1518,7 +1527,7 @@
       </c>
       <c r="D108" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -1527,7 +1536,7 @@
       </c>
       <c r="D109" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -1536,7 +1545,7 @@
       </c>
       <c r="D110" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -1545,7 +1554,7 @@
       </c>
       <c r="D111" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -1554,7 +1563,7 @@
       </c>
       <c r="D112" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -1563,7 +1572,7 @@
       </c>
       <c r="D113" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -1572,7 +1581,7 @@
       </c>
       <c r="D114" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -1581,7 +1590,7 @@
       </c>
       <c r="D115" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -1590,7 +1599,7 @@
       </c>
       <c r="D116" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -1599,7 +1608,7 @@
       </c>
       <c r="D117" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -1608,7 +1617,7 @@
       </c>
       <c r="D118" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -1617,7 +1626,7 @@
       </c>
       <c r="D119" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -1626,7 +1635,7 @@
       </c>
       <c r="D120" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -1635,7 +1644,7 @@
       </c>
       <c r="D121" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -1644,7 +1653,7 @@
       </c>
       <c r="D122" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -1653,7 +1662,7 @@
       </c>
       <c r="D123" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -1662,7 +1671,7 @@
       </c>
       <c r="D124" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -1671,7 +1680,7 @@
       </c>
       <c r="D125" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -1680,7 +1689,7 @@
       </c>
       <c r="D126" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -1689,7 +1698,7 @@
       </c>
       <c r="D127" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -5359,11 +5368,11 @@
       </c>
       <c r="B7" s="1">
         <f>SUM('1_Mateusz_Skrzypek'!B7,'2_Imię_Nazwisko'!B7,'4_Imię_Nazwisko'!B7)</f>
-        <v>5</v>
+        <v>8.5</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5372,11 +5381,11 @@
       </c>
       <c r="B8" s="1">
         <f>SUM('1_Mateusz_Skrzypek'!B8,'2_Imię_Nazwisko'!B8,'4_Imię_Nazwisko'!B8)</f>
-        <v>0</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5389,7 +5398,7 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5402,7 +5411,7 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5415,7 +5424,7 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5428,7 +5437,7 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5441,7 +5450,7 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5454,7 +5463,7 @@
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -5467,7 +5476,7 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -5480,7 +5489,7 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5493,7 +5502,7 @@
       </c>
       <c r="C17" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -5506,7 +5515,7 @@
       </c>
       <c r="C18" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5519,7 +5528,7 @@
       </c>
       <c r="C19" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5532,7 +5541,7 @@
       </c>
       <c r="C20" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -5545,7 +5554,7 @@
       </c>
       <c r="C21" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -5558,7 +5567,7 @@
       </c>
       <c r="C22" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5571,7 +5580,7 @@
       </c>
       <c r="C23" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -5584,7 +5593,7 @@
       </c>
       <c r="C24" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -5597,7 +5606,7 @@
       </c>
       <c r="C25" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -5610,7 +5619,7 @@
       </c>
       <c r="C26" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -5623,7 +5632,7 @@
       </c>
       <c r="C27" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -5636,7 +5645,7 @@
       </c>
       <c r="C28" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -5649,7 +5658,7 @@
       </c>
       <c r="C29" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -5662,7 +5671,7 @@
       </c>
       <c r="C30" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -5675,7 +5684,7 @@
       </c>
       <c r="C31" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -5688,7 +5697,7 @@
       </c>
       <c r="C32" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -5701,7 +5710,7 @@
       </c>
       <c r="C33" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5714,7 +5723,7 @@
       </c>
       <c r="C34" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -5727,7 +5736,7 @@
       </c>
       <c r="C35" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -5740,7 +5749,7 @@
       </c>
       <c r="C36" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5753,7 +5762,7 @@
       </c>
       <c r="C37" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -5766,7 +5775,7 @@
       </c>
       <c r="C38" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5779,7 +5788,7 @@
       </c>
       <c r="C39" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5792,7 +5801,7 @@
       </c>
       <c r="C40" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -5805,7 +5814,7 @@
       </c>
       <c r="C41" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5818,7 +5827,7 @@
       </c>
       <c r="C42" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -5831,7 +5840,7 @@
       </c>
       <c r="C43" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -5844,7 +5853,7 @@
       </c>
       <c r="C44" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -5857,7 +5866,7 @@
       </c>
       <c r="C45" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -5870,7 +5879,7 @@
       </c>
       <c r="C46" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -5883,7 +5892,7 @@
       </c>
       <c r="C47" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -5896,7 +5905,7 @@
       </c>
       <c r="C48" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -5909,7 +5918,7 @@
       </c>
       <c r="C49" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -5922,7 +5931,7 @@
       </c>
       <c r="C50" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5935,7 +5944,7 @@
       </c>
       <c r="C51" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -5948,7 +5957,7 @@
       </c>
       <c r="C52" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5961,7 +5970,7 @@
       </c>
       <c r="C53" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -5974,7 +5983,7 @@
       </c>
       <c r="C54" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5987,7 +5996,7 @@
       </c>
       <c r="C55" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -6000,7 +6009,7 @@
       </c>
       <c r="C56" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -6013,7 +6022,7 @@
       </c>
       <c r="C57" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -6026,7 +6035,7 @@
       </c>
       <c r="C58" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -6039,7 +6048,7 @@
       </c>
       <c r="C59" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -6052,7 +6061,7 @@
       </c>
       <c r="C60" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -6065,7 +6074,7 @@
       </c>
       <c r="C61" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -6078,7 +6087,7 @@
       </c>
       <c r="C62" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -6091,7 +6100,7 @@
       </c>
       <c r="C63" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -6104,7 +6113,7 @@
       </c>
       <c r="C64" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -6117,7 +6126,7 @@
       </c>
       <c r="C65" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -6130,7 +6139,7 @@
       </c>
       <c r="C66" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6143,7 +6152,7 @@
       </c>
       <c r="C67" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -6156,7 +6165,7 @@
       </c>
       <c r="C68" s="1">
         <f t="shared" ref="C68:C127" si="1">C67+B68</f>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -6169,7 +6178,7 @@
       </c>
       <c r="C69" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -6182,7 +6191,7 @@
       </c>
       <c r="C70" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -6195,7 +6204,7 @@
       </c>
       <c r="C71" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -6208,7 +6217,7 @@
       </c>
       <c r="C72" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -6221,7 +6230,7 @@
       </c>
       <c r="C73" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -6234,7 +6243,7 @@
       </c>
       <c r="C74" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -6247,7 +6256,7 @@
       </c>
       <c r="C75" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -6260,7 +6269,7 @@
       </c>
       <c r="C76" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -6273,7 +6282,7 @@
       </c>
       <c r="C77" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -6286,7 +6295,7 @@
       </c>
       <c r="C78" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -6299,7 +6308,7 @@
       </c>
       <c r="C79" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -6312,7 +6321,7 @@
       </c>
       <c r="C80" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -6325,7 +6334,7 @@
       </c>
       <c r="C81" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -6338,7 +6347,7 @@
       </c>
       <c r="C82" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -6351,7 +6360,7 @@
       </c>
       <c r="C83" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -6364,7 +6373,7 @@
       </c>
       <c r="C84" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -6377,7 +6386,7 @@
       </c>
       <c r="C85" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -6390,7 +6399,7 @@
       </c>
       <c r="C86" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -6403,7 +6412,7 @@
       </c>
       <c r="C87" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -6416,7 +6425,7 @@
       </c>
       <c r="C88" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -6429,7 +6438,7 @@
       </c>
       <c r="C89" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -6442,7 +6451,7 @@
       </c>
       <c r="C90" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -6455,7 +6464,7 @@
       </c>
       <c r="C91" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -6468,7 +6477,7 @@
       </c>
       <c r="C92" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -6481,7 +6490,7 @@
       </c>
       <c r="C93" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -6494,7 +6503,7 @@
       </c>
       <c r="C94" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -6507,7 +6516,7 @@
       </c>
       <c r="C95" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -6520,7 +6529,7 @@
       </c>
       <c r="C96" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -6533,7 +6542,7 @@
       </c>
       <c r="C97" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -6546,7 +6555,7 @@
       </c>
       <c r="C98" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -6559,7 +6568,7 @@
       </c>
       <c r="C99" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -6572,7 +6581,7 @@
       </c>
       <c r="C100" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -6585,7 +6594,7 @@
       </c>
       <c r="C101" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -6598,7 +6607,7 @@
       </c>
       <c r="C102" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -6611,7 +6620,7 @@
       </c>
       <c r="C103" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -6624,7 +6633,7 @@
       </c>
       <c r="C104" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -6637,7 +6646,7 @@
       </c>
       <c r="C105" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -6650,7 +6659,7 @@
       </c>
       <c r="C106" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -6663,7 +6672,7 @@
       </c>
       <c r="C107" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -6676,7 +6685,7 @@
       </c>
       <c r="C108" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -6689,7 +6698,7 @@
       </c>
       <c r="C109" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -6702,7 +6711,7 @@
       </c>
       <c r="C110" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -6715,7 +6724,7 @@
       </c>
       <c r="C111" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -6728,7 +6737,7 @@
       </c>
       <c r="C112" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -6741,7 +6750,7 @@
       </c>
       <c r="C113" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -6754,7 +6763,7 @@
       </c>
       <c r="C114" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -6767,7 +6776,7 @@
       </c>
       <c r="C115" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -6780,7 +6789,7 @@
       </c>
       <c r="C116" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -6793,7 +6802,7 @@
       </c>
       <c r="C117" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -6806,7 +6815,7 @@
       </c>
       <c r="C118" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -6819,7 +6828,7 @@
       </c>
       <c r="C119" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -6832,7 +6841,7 @@
       </c>
       <c r="C120" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -6845,7 +6854,7 @@
       </c>
       <c r="C121" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -6858,7 +6867,7 @@
       </c>
       <c r="C122" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -6871,7 +6880,7 @@
       </c>
       <c r="C123" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -6884,7 +6893,7 @@
       </c>
       <c r="C124" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -6897,7 +6906,7 @@
       </c>
       <c r="C125" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -6910,7 +6919,7 @@
       </c>
       <c r="C126" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -6923,7 +6932,7 @@
       </c>
       <c r="C127" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -6947,6 +6956,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BF63F47345AA104BAD8025403A332EC4" ma:contentTypeVersion="4" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="2b9be556d413d7c3e99fff097a4a98c2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="880b73d8-af7f-42e3-972b-e46fe4ffca1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="643da98f93f748be063e7f29d6c7d305" ns2:_="">
     <xsd:import namespace="880b73d8-af7f-42e3-972b-e46fe4ffca1b"/>
@@ -7090,22 +7114,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6570E11-21DF-40C1-8E5B-FD3CDF32C4F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21938D86-7413-468E-85B7-E79A45C27865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57B575B8-240F-4CC3-A552-189C22DB0968}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7121,21 +7147,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21938D86-7413-468E-85B7-E79A45C27865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6570E11-21DF-40C1-8E5B-FD3CDF32C4F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>